<commit_message>
corrected story points from 18 to 21
</commit_message>
<xml_diff>
--- a/Reference Stories.xlsx
+++ b/Reference Stories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ansuman\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A97FAB2-6501-4488-BAC9-A17391F0585C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12825BFF-FE7B-41F3-AE6B-1548ADA410A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E533CDD9-535F-4D8B-96CB-D169F5142949}"/>
   </bookViews>
@@ -327,13 +327,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0019EF26-1D52-451B-B262-54D9254FF84C}" name="Table1" displayName="Table1" ref="B2:E23" totalsRowShown="0" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0019EF26-1D52-451B-B262-54D9254FF84C}" name="Table1" displayName="Table1" ref="B2:E23" totalsRowShown="0" dataDxfId="4">
   <autoFilter ref="B2:E23" xr:uid="{0019EF26-1D52-451B-B262-54D9254FF84C}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{FF98576D-71EA-4B31-9380-D85F2D8A1CE4}" name="Reference Story No." dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{63043FAD-DF60-44E3-914B-89AFF1594CAE}" name="Pool" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{0112A55E-05F3-47D2-81B7-54C2270AAB56}" name="Source" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{5577F3C4-C435-4C95-9D19-381EA4D7D48B}" name="Story Summary" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{FF98576D-71EA-4B31-9380-D85F2D8A1CE4}" name="Reference Story No." dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{63043FAD-DF60-44E3-914B-89AFF1594CAE}" name="Pool" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{0112A55E-05F3-47D2-81B7-54C2270AAB56}" name="Source" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{5577F3C4-C435-4C95-9D19-381EA4D7D48B}" name="Story Summary" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -658,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCC3D2D9-C285-45A9-92A0-89252FBB9997}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -945,7 +945,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="2">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>16</v>
@@ -959,7 +959,7 @@
         <v>20</v>
       </c>
       <c r="C22" s="2">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>20</v>
@@ -973,7 +973,7 @@
         <v>21</v>
       </c>
       <c r="C23" s="2">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>12</v>

</xml_diff>